<commit_message>
Fixed Headings to adjust around 0 and 360 degrees
E.g when TC is 5 deg and MV is -13 deg, the MC would show -8 deg, which should have been 352 deg, this is fixed now.
</commit_message>
<xml_diff>
--- a/vaayuyaana/jagiNavLog.xlsx
+++ b/vaayuyaana/jagiNavLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagadishn\Documents\jagi\haaru\aerodynamic\stage03\XC\dual\xc02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagadishn\Documents\jagi\haaru\aerodynamic\stage03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E6C763-0951-4080-9C02-BD7A4341BAC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B7725B-64BC-44DB-AE40-CCE6160331E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3DE2A8C-E23C-4F63-95E8-9AD5B4E402C0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E3DE2A8C-E23C-4F63-95E8-9AD5B4E402C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -988,19 +988,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1032,7 +1019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1190,11 +1177,110 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1202,28 +1288,88 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1232,205 +1378,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1830,7 +1823,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,35 +1839,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="105"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="103"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="135" t="s">
+      <c r="R1" s="104" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="106"/>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="107"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="106"/>
     </row>
     <row r="2" spans="1:23" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1892,219 +1885,219 @@
       <c r="G2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="134"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="70"/>
       <c r="J2" s="4" t="s">
         <v>74</v>
       </c>
       <c r="K2" s="3"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="96"/>
-      <c r="V2" s="96"/>
-      <c r="W2" s="132"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="63"/>
     </row>
     <row r="3" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="130" t="s">
+      <c r="A3" s="93"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130" t="s">
+      <c r="E3" s="68"/>
+      <c r="F3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130" t="s">
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="99"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="64"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
       <c r="J4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="99"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="64"/>
     </row>
     <row r="5" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="117"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="97"/>
-      <c r="R5" s="97"/>
-      <c r="S5" s="97"/>
-      <c r="T5" s="97"/>
-      <c r="U5" s="97"/>
-      <c r="V5" s="97"/>
-      <c r="W5" s="99"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="60"/>
+      <c r="W5" s="64"/>
     </row>
     <row r="6" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
       <c r="J6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97"/>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="97"/>
-      <c r="R6" s="97"/>
-      <c r="S6" s="97"/>
-      <c r="T6" s="97"/>
-      <c r="U6" s="97"/>
-      <c r="V6" s="97"/>
-      <c r="W6" s="99"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="60"/>
+      <c r="V6" s="60"/>
+      <c r="W6" s="64"/>
     </row>
     <row r="7" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
       <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="97"/>
-      <c r="T7" s="97"/>
-      <c r="U7" s="97"/>
-      <c r="V7" s="97"/>
-      <c r="W7" s="99"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="60"/>
+      <c r="W7" s="64"/>
     </row>
     <row r="8" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
       <c r="J8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="131"/>
-      <c r="L8" s="131"/>
-      <c r="M8" s="131"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
-      <c r="S8" s="88"/>
-      <c r="T8" s="88"/>
-      <c r="U8" s="88"/>
-      <c r="V8" s="88"/>
-      <c r="W8" s="89"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="61"/>
+      <c r="T8" s="61"/>
+      <c r="U8" s="61"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="65"/>
     </row>
     <row r="9" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="87"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="124" t="s">
+      <c r="D9" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="127" t="s">
+      <c r="E9" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="86"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="42" t="s">
         <v>85</v>
       </c>
@@ -2117,7 +2110,7 @@
       <c r="K9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="87" t="s">
+      <c r="L9" s="57" t="s">
         <v>24</v>
       </c>
       <c r="M9" s="28" t="s">
@@ -2126,34 +2119,34 @@
       <c r="N9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="86" t="s">
+      <c r="O9" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="86"/>
+      <c r="P9" s="55"/>
       <c r="Q9" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="85" t="s">
+      <c r="R9" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="S9" s="86"/>
-      <c r="T9" s="115" t="s">
+      <c r="S9" s="55"/>
+      <c r="T9" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="U9" s="86"/>
-      <c r="V9" s="86" t="s">
+      <c r="U9" s="55"/>
+      <c r="V9" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="W9" s="87"/>
+      <c r="W9" s="57"/>
     </row>
     <row r="10" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="122"/>
-      <c r="B10" s="123"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="125"/>
-      <c r="E10" s="128"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="9" t="s">
         <v>17</v>
       </c>
@@ -2163,58 +2156,58 @@
       <c r="H10" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="118" t="s">
+      <c r="I10" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="118" t="s">
+      <c r="J10" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="120" t="s">
+      <c r="K10" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="123"/>
+      <c r="L10" s="58"/>
       <c r="M10" s="9" t="s">
         <v>28</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
       <c r="Q10" s="41" t="str">
         <f>IF(ISNUMBER(I34),I34,"")</f>
         <v/>
       </c>
-      <c r="R10" s="80"/>
-      <c r="S10" s="81"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="95"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="97"/>
+      <c r="T10" s="97"/>
+      <c r="U10" s="97"/>
+      <c r="V10" s="97"/>
+      <c r="W10" s="59"/>
     </row>
     <row r="11" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
-      <c r="B11" s="95"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="125"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="98" t="s">
+      <c r="D11" s="85"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="97"/>
-      <c r="H11" s="63" t="s">
+      <c r="G11" s="60"/>
+      <c r="H11" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="123"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="58"/>
       <c r="M11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="97" t="s">
+      <c r="N11" s="60" t="s">
         <v>32</v>
       </c>
       <c r="O11" s="10" t="s">
@@ -2226,30 +2219,30 @@
       <c r="Q11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="R11" s="82"/>
-      <c r="S11" s="83"/>
-      <c r="T11" s="96" t="s">
+      <c r="R11" s="114"/>
+      <c r="S11" s="115"/>
+      <c r="T11" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="U11" s="96"/>
-      <c r="V11" s="83"/>
-      <c r="W11" s="84"/>
+      <c r="U11" s="62"/>
+      <c r="V11" s="115"/>
+      <c r="W11" s="118"/>
     </row>
     <row r="12" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="110"/>
-      <c r="B12" s="132"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="129"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="121"/>
-      <c r="L12" s="95"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="59"/>
       <c r="M12" s="36"/>
-      <c r="N12" s="88"/>
+      <c r="N12" s="61"/>
       <c r="O12" s="14" t="s">
         <v>34</v>
       </c>
@@ -2259,38 +2252,38 @@
       <c r="Q12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="R12" s="93"/>
-      <c r="S12" s="76"/>
-      <c r="T12" s="97" t="s">
+      <c r="R12" s="116"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="U12" s="97"/>
-      <c r="V12" s="76"/>
-      <c r="W12" s="77"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="56"/>
+      <c r="W12" s="119"/>
     </row>
     <row r="13" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
-      <c r="B13" s="99"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="30"/>
-      <c r="D13" s="73" t="str">
-        <f t="shared" ref="D13:D15" si="0">IF(I13&lt;&gt;"",I13+J14,"")</f>
-        <v/>
-      </c>
-      <c r="E13" s="92"/>
+      <c r="D13" s="108" t="str">
+        <f>IF(I13&lt;&gt;"",MOD(I13+J14,360),"")</f>
+        <v/>
+      </c>
+      <c r="E13" s="125"/>
       <c r="F13" s="34"/>
       <c r="G13" s="31"/>
-      <c r="H13" s="109"/>
+      <c r="H13" s="111"/>
       <c r="I13" s="31"/>
-      <c r="J13" s="49" t="str">
-        <f>IF(I13&lt;&gt;"",IF(ISNUMBER(I14),I13+I14,I13),"")</f>
-        <v/>
-      </c>
-      <c r="K13" s="49" t="str">
-        <f>IF(J13&lt;&gt;"",J13+J14,"")</f>
-        <v/>
-      </c>
-      <c r="L13" s="59" t="str">
-        <f>IF(K13&lt;&gt;"",K13+K14,"")</f>
+      <c r="J13" s="47" t="str">
+        <f>IF(I13&lt;&gt;"",IF(ISNUMBER(I14),MOD(I13+I14,360),I13),"")</f>
+        <v/>
+      </c>
+      <c r="K13" s="47" t="str">
+        <f>IF(J13&lt;&gt;"",MOD(J13+J14,360),"")</f>
+        <v/>
+      </c>
+      <c r="L13" s="128" t="str">
+        <f>IF(K13&lt;&gt;"",MOD(K13+K14,360),"")</f>
         <v/>
       </c>
       <c r="M13" s="34"/>
@@ -2307,31 +2300,31 @@
         <f>IF(ISNUMBER(O13),$L$34+O13*$Q$10/60,"")</f>
         <v/>
       </c>
-      <c r="R13" s="93"/>
-      <c r="S13" s="76"/>
-      <c r="T13" s="97" t="s">
+      <c r="R13" s="116"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="U13" s="97"/>
-      <c r="V13" s="76"/>
-      <c r="W13" s="77"/>
+      <c r="U13" s="60"/>
+      <c r="V13" s="56"/>
+      <c r="W13" s="119"/>
     </row>
-    <row r="14" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="98"/>
-      <c r="B14" s="99"/>
+    <row r="14" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="71"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="30"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="58"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="91"/>
       <c r="I14" s="47" t="str">
         <f>IF(F13&lt;&gt;"",DEGREES(ASIN(G13/H13*SIN(RADIANS(F13-I13)))),"")</f>
         <v/>
       </c>
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
-      <c r="L14" s="60"/>
+      <c r="L14" s="129"/>
       <c r="M14" s="44" t="str">
         <f>IF(ISNUMBER(M13),M12-M13,"")</f>
         <v/>
@@ -2343,38 +2336,38 @@
         <f>IF(AND(ISNUMBER(Q34),ISNUMBER(Q13)),Q34-L34-Q13,"")</f>
         <v/>
       </c>
-      <c r="R14" s="93"/>
-      <c r="S14" s="76"/>
-      <c r="T14" s="97" t="s">
+      <c r="R14" s="116"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="U14" s="97"/>
-      <c r="V14" s="76"/>
-      <c r="W14" s="77"/>
+      <c r="U14" s="60"/>
+      <c r="V14" s="56"/>
+      <c r="W14" s="119"/>
     </row>
     <row r="15" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="98"/>
-      <c r="B15" s="99"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="30"/>
-      <c r="D15" s="73" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E15" s="75"/>
+      <c r="D15" s="108" t="str">
+        <f>IF(I15&lt;&gt;"",MOD(I15+J16,360),"")</f>
+        <v/>
+      </c>
+      <c r="E15" s="110"/>
       <c r="F15" s="35"/>
       <c r="G15" s="32"/>
-      <c r="H15" s="57"/>
+      <c r="H15" s="90"/>
       <c r="I15" s="32"/>
       <c r="J15" s="47" t="str">
-        <f>IF(I15&lt;&gt;"",IF(ISNUMBER(I16),I15+I16,I15),"")</f>
+        <f>IF(I15&lt;&gt;"",IF(ISNUMBER(I16),MOD(I15+I16,360),I15),"")</f>
         <v/>
       </c>
       <c r="K15" s="47" t="str">
-        <f>IF(J15&lt;&gt;"",J15+J16,"")</f>
-        <v/>
-      </c>
-      <c r="L15" s="61" t="str">
-        <f>IF(K15&lt;&gt;"",K15+K16,"")</f>
+        <f>IF(J15&lt;&gt;"",MOD(J15+J16,360),"")</f>
+        <v/>
+      </c>
+      <c r="L15" s="128" t="str">
+        <f>IF(K15&lt;&gt;"",MOD(K15+K16,360),"")</f>
         <v/>
       </c>
       <c r="M15" s="35"/>
@@ -2391,31 +2384,31 @@
         <f>IF(ISNUMBER(O15),O15*$Q$10/60,"")</f>
         <v/>
       </c>
-      <c r="R15" s="93"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="97" t="s">
+      <c r="R15" s="116"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="U15" s="97"/>
-      <c r="V15" s="76"/>
-      <c r="W15" s="77"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="119"/>
     </row>
-    <row r="16" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
-      <c r="B16" s="99"/>
+    <row r="16" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="71"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="30"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="58"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="99"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="91"/>
       <c r="I16" s="47" t="str">
         <f>IF(F15&lt;&gt;"",DEGREES(ASIN(G15/H15*SIN(RADIANS(F15-I15)))),"")</f>
         <v/>
       </c>
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
-      <c r="L16" s="60"/>
+      <c r="L16" s="129"/>
       <c r="M16" s="44" t="str">
         <f>IF(ISNUMBER(M15),M14-M15,"")</f>
         <v/>
@@ -2427,38 +2420,38 @@
         <f>IF(AND(ISNUMBER(Q14),ISNUMBER(Q15)),Q14-Q15,"")</f>
         <v/>
       </c>
-      <c r="R16" s="93"/>
-      <c r="S16" s="76"/>
-      <c r="T16" s="97" t="s">
+      <c r="R16" s="116"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="U16" s="97"/>
-      <c r="V16" s="76"/>
-      <c r="W16" s="77"/>
+      <c r="U16" s="60"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="119"/>
     </row>
     <row r="17" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="98"/>
-      <c r="B17" s="99"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="64"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="73" t="str">
-        <f>IF(I17&lt;&gt;"",I17+J18,"")</f>
-        <v/>
-      </c>
-      <c r="E17" s="75"/>
+      <c r="D17" s="108" t="str">
+        <f>IF(I17&lt;&gt;"",MOD(I17+J18,360),"")</f>
+        <v/>
+      </c>
+      <c r="E17" s="110"/>
       <c r="F17" s="35"/>
       <c r="G17" s="32"/>
-      <c r="H17" s="57"/>
+      <c r="H17" s="90"/>
       <c r="I17" s="32"/>
       <c r="J17" s="47" t="str">
-        <f>IF(I17&lt;&gt;"",IF(ISNUMBER(I18),I17+I18,I17),"")</f>
+        <f>IF(I17&lt;&gt;"",IF(ISNUMBER(I18),MOD(I17+I18,360),I17),"")</f>
         <v/>
       </c>
       <c r="K17" s="47" t="str">
-        <f>IF(J17&lt;&gt;"",J17+J18,"")</f>
-        <v/>
-      </c>
-      <c r="L17" s="61" t="str">
-        <f>IF(K17&lt;&gt;"",K17+K18,"")</f>
+        <f>IF(J17&lt;&gt;"",MOD(J17+J18,360),"")</f>
+        <v/>
+      </c>
+      <c r="L17" s="128" t="str">
+        <f>IF(K17&lt;&gt;"",MOD(K17+K18,360),"")</f>
         <v/>
       </c>
       <c r="M17" s="35"/>
@@ -2475,31 +2468,31 @@
         <f>IF(ISNUMBER(O17),O17*$Q$10/60,"")</f>
         <v/>
       </c>
-      <c r="R17" s="94"/>
-      <c r="S17" s="78"/>
+      <c r="R17" s="117"/>
+      <c r="S17" s="112"/>
       <c r="T17" s="100" t="s">
         <v>45</v>
       </c>
       <c r="U17" s="100"/>
-      <c r="V17" s="78"/>
-      <c r="W17" s="79"/>
+      <c r="V17" s="112"/>
+      <c r="W17" s="113"/>
     </row>
-    <row r="18" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="98"/>
-      <c r="B18" s="99"/>
+    <row r="18" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="71"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="58"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="91"/>
       <c r="I18" s="47" t="str">
         <f>IF(F17&lt;&gt;"",DEGREES(ASIN(G17/H17*SIN(RADIANS(F17-I17)))),"")</f>
         <v/>
       </c>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
-      <c r="L18" s="60"/>
+      <c r="L18" s="129"/>
       <c r="M18" s="44" t="str">
         <f>IF(ISNUMBER(M17),M16-M17,"")</f>
         <v/>
@@ -2519,28 +2512,28 @@
       <c r="W18" s="17"/>
     </row>
     <row r="19" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="98"/>
-      <c r="B19" s="99"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="30"/>
-      <c r="D19" s="73" t="str">
-        <f>IF(I19&lt;&gt;"",I19+J20,"")</f>
-        <v/>
-      </c>
-      <c r="E19" s="75"/>
+      <c r="D19" s="108" t="str">
+        <f>IF(I19&lt;&gt;"",MOD(I19+J20,360),"")</f>
+        <v/>
+      </c>
+      <c r="E19" s="110"/>
       <c r="F19" s="35"/>
       <c r="G19" s="32"/>
-      <c r="H19" s="57"/>
+      <c r="H19" s="90"/>
       <c r="I19" s="32"/>
       <c r="J19" s="47" t="str">
-        <f>IF(I19&lt;&gt;"",IF(ISNUMBER(I20),I19+I20,I19),"")</f>
+        <f>IF(I19&lt;&gt;"",IF(ISNUMBER(I20),MOD(I19+I20,360),I19),"")</f>
         <v/>
       </c>
       <c r="K19" s="47" t="str">
-        <f>IF(J19&lt;&gt;"",J19+J20,"")</f>
-        <v/>
-      </c>
-      <c r="L19" s="61" t="str">
-        <f>IF(K19&lt;&gt;"",K19+K20,"")</f>
+        <f>IF(J19&lt;&gt;"",MOD(J19+J20,360),"")</f>
+        <v/>
+      </c>
+      <c r="L19" s="128" t="str">
+        <f>IF(K19&lt;&gt;"",MOD(K19+K20,360),"")</f>
         <v/>
       </c>
       <c r="M19" s="35"/>
@@ -2565,21 +2558,21 @@
       <c r="W19" s="19"/>
     </row>
     <row r="20" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="98"/>
-      <c r="B20" s="99"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="30"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="58"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="91"/>
       <c r="I20" s="47" t="str">
         <f>IF(F19&lt;&gt;"",DEGREES(ASIN(G19/H19*SIN(RADIANS(F19-I19)))),"")</f>
         <v/>
       </c>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
-      <c r="L20" s="60"/>
+      <c r="L20" s="129"/>
       <c r="M20" s="44" t="str">
         <f>IF(ISNUMBER(M19),M18-M19,"")</f>
         <v/>
@@ -2599,28 +2592,28 @@
       <c r="W20" s="19"/>
     </row>
     <row r="21" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="98"/>
-      <c r="B21" s="99"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="30"/>
-      <c r="D21" s="73" t="str">
-        <f t="shared" ref="D21" si="1">IF(I21&lt;&gt;"",I21+J22,"")</f>
-        <v/>
-      </c>
-      <c r="E21" s="75"/>
+      <c r="D21" s="108" t="str">
+        <f>IF(I21&lt;&gt;"",MOD(I21+J22,360),"")</f>
+        <v/>
+      </c>
+      <c r="E21" s="110"/>
       <c r="F21" s="35"/>
       <c r="G21" s="32"/>
-      <c r="H21" s="57"/>
+      <c r="H21" s="90"/>
       <c r="I21" s="32"/>
       <c r="J21" s="47" t="str">
-        <f>IF(I21&lt;&gt;"",IF(ISNUMBER(I22),I21+I22,I21),"")</f>
+        <f>IF(I21&lt;&gt;"",IF(ISNUMBER(I22),MOD(I21+I22,360),I21),"")</f>
         <v/>
       </c>
       <c r="K21" s="47" t="str">
-        <f>IF(J21&lt;&gt;"",J21+J22,"")</f>
-        <v/>
-      </c>
-      <c r="L21" s="61" t="str">
-        <f t="shared" ref="L21" si="2">IF(K21&lt;&gt;"",K21+K22,"")</f>
+        <f>IF(J21&lt;&gt;"",MOD(J21+J22,360),"")</f>
+        <v/>
+      </c>
+      <c r="L21" s="128" t="str">
+        <f>IF(K21&lt;&gt;"",MOD(K21+K22,360),"")</f>
         <v/>
       </c>
       <c r="M21" s="35"/>
@@ -2637,31 +2630,31 @@
         <f>IF(ISNUMBER(O21),O21*$Q$10/60,"")</f>
         <v/>
       </c>
-      <c r="R21" s="85" t="s">
+      <c r="R21" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="S21" s="86"/>
-      <c r="T21" s="86"/>
-      <c r="U21" s="86"/>
-      <c r="V21" s="86"/>
-      <c r="W21" s="87"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="57"/>
     </row>
     <row r="22" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="98"/>
-      <c r="B22" s="99"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="64"/>
       <c r="C22" s="30"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="58"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="91"/>
       <c r="I22" s="47" t="str">
         <f>IF(F21&lt;&gt;"",DEGREES(ASIN(G21/H21*SIN(RADIANS(F21-I21)))),"")</f>
         <v/>
       </c>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
-      <c r="L22" s="60"/>
+      <c r="L22" s="129"/>
       <c r="M22" s="44" t="str">
         <f>IF(ISNUMBER(M21),M20-M21,"")</f>
         <v/>
@@ -2673,40 +2666,40 @@
         <f>IF(AND(ISNUMBER(Q20),ISNUMBER(Q21)),Q20-Q21,"")</f>
         <v/>
       </c>
-      <c r="R22" s="80" t="s">
+      <c r="R22" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="S22" s="81"/>
-      <c r="T22" s="81"/>
-      <c r="U22" s="81" t="s">
+      <c r="S22" s="97"/>
+      <c r="T22" s="97"/>
+      <c r="U22" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="V22" s="81"/>
-      <c r="W22" s="95"/>
+      <c r="V22" s="97"/>
+      <c r="W22" s="59"/>
     </row>
     <row r="23" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="98"/>
-      <c r="B23" s="99"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="64"/>
       <c r="C23" s="30"/>
-      <c r="D23" s="73" t="str">
-        <f t="shared" ref="D23" si="3">IF(I23&lt;&gt;"",I23+J24,"")</f>
-        <v/>
-      </c>
-      <c r="E23" s="75"/>
+      <c r="D23" s="108" t="str">
+        <f>IF(I23&lt;&gt;"",MOD(I23+J24,360),"")</f>
+        <v/>
+      </c>
+      <c r="E23" s="110"/>
       <c r="F23" s="35"/>
       <c r="G23" s="32"/>
-      <c r="H23" s="57"/>
+      <c r="H23" s="90"/>
       <c r="I23" s="32"/>
       <c r="J23" s="47" t="str">
-        <f>IF(I23&lt;&gt;"",IF(ISNUMBER(I24),I23+I24,I23),"")</f>
+        <f>IF(I23&lt;&gt;"",IF(ISNUMBER(I24),MOD(I23+I24,360),I23),"")</f>
         <v/>
       </c>
       <c r="K23" s="47" t="str">
-        <f>IF(J23&lt;&gt;"",J23+J24,"")</f>
-        <v/>
-      </c>
-      <c r="L23" s="61" t="str">
-        <f t="shared" ref="L23" si="4">IF(K23&lt;&gt;"",K23+K24,"")</f>
+        <f>IF(J23&lt;&gt;"",MOD(J23+J24,360),"")</f>
+        <v/>
+      </c>
+      <c r="L23" s="128" t="str">
+        <f>IF(K23&lt;&gt;"",MOD(K23+K24,360),"")</f>
         <v/>
       </c>
       <c r="M23" s="35"/>
@@ -2723,29 +2716,29 @@
         <f>IF(ISNUMBER(O23),O23*$Q$10/60,"")</f>
         <v/>
       </c>
-      <c r="R23" s="82"/>
-      <c r="S23" s="83"/>
-      <c r="T23" s="83"/>
-      <c r="U23" s="83"/>
-      <c r="V23" s="83"/>
-      <c r="W23" s="84"/>
+      <c r="R23" s="114"/>
+      <c r="S23" s="115"/>
+      <c r="T23" s="115"/>
+      <c r="U23" s="115"/>
+      <c r="V23" s="115"/>
+      <c r="W23" s="118"/>
     </row>
-    <row r="24" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="98"/>
-      <c r="B24" s="99"/>
+    <row r="24" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="71"/>
+      <c r="B24" s="64"/>
       <c r="C24" s="30"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="58"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="91"/>
       <c r="I24" s="47" t="str">
         <f>IF(F23&lt;&gt;"",DEGREES(ASIN(G23/H23*SIN(RADIANS(F23-I23)))),"")</f>
         <v/>
       </c>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
-      <c r="L24" s="60"/>
+      <c r="L24" s="129"/>
       <c r="M24" s="44" t="str">
         <f>IF(ISNUMBER(M23),M22-M23,"")</f>
         <v/>
@@ -2760,37 +2753,37 @@
       <c r="R24" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="S24" s="76"/>
-      <c r="T24" s="76"/>
+      <c r="S24" s="134"/>
+      <c r="T24" s="134"/>
       <c r="U24" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="V24" s="76"/>
-      <c r="W24" s="77"/>
+      <c r="V24" s="134"/>
+      <c r="W24" s="136"/>
     </row>
     <row r="25" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="98"/>
-      <c r="B25" s="99"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="64"/>
       <c r="C25" s="30"/>
-      <c r="D25" s="73" t="str">
-        <f t="shared" ref="D25" si="5">IF(I25&lt;&gt;"",I25+J26,"")</f>
-        <v/>
-      </c>
-      <c r="E25" s="75"/>
+      <c r="D25" s="108" t="str">
+        <f>IF(I25&lt;&gt;"",MOD(I25+J26,360),"")</f>
+        <v/>
+      </c>
+      <c r="E25" s="110"/>
       <c r="F25" s="35"/>
       <c r="G25" s="32"/>
-      <c r="H25" s="57"/>
+      <c r="H25" s="90"/>
       <c r="I25" s="32"/>
       <c r="J25" s="47" t="str">
-        <f>IF(I25&lt;&gt;"",IF(ISNUMBER(I26),I25+I26,I25),"")</f>
+        <f>IF(I25&lt;&gt;"",IF(ISNUMBER(I26),MOD(I25+I26,360),I25),"")</f>
         <v/>
       </c>
       <c r="K25" s="47" t="str">
-        <f>IF(J25&lt;&gt;"",J25+J26,"")</f>
-        <v/>
-      </c>
-      <c r="L25" s="61" t="str">
-        <f t="shared" ref="L25" si="6">IF(K25&lt;&gt;"",K25+K26,"")</f>
+        <f>IF(J25&lt;&gt;"",MOD(J25+J26,360),"")</f>
+        <v/>
+      </c>
+      <c r="L25" s="128" t="str">
+        <f>IF(K25&lt;&gt;"",MOD(K25+K26,360),"")</f>
         <v/>
       </c>
       <c r="M25" s="35"/>
@@ -2810,30 +2803,30 @@
       <c r="R25" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="S25" s="76"/>
-      <c r="T25" s="76"/>
+      <c r="S25" s="134"/>
+      <c r="T25" s="134"/>
       <c r="U25" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="V25" s="76"/>
-      <c r="W25" s="77"/>
+      <c r="V25" s="134"/>
+      <c r="W25" s="136"/>
     </row>
-    <row r="26" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="98"/>
-      <c r="B26" s="99"/>
+    <row r="26" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="71"/>
+      <c r="B26" s="64"/>
       <c r="C26" s="30"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="58"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="99"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="91"/>
       <c r="I26" s="47" t="str">
         <f>IF(F25&lt;&gt;"",DEGREES(ASIN(G25/H25*SIN(RADIANS(F25-I25)))),"")</f>
         <v/>
       </c>
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
-      <c r="L26" s="60"/>
+      <c r="L26" s="129"/>
       <c r="M26" s="44" t="str">
         <f>IF(ISNUMBER(M25),M24-M25,"")</f>
         <v/>
@@ -2848,37 +2841,37 @@
       <c r="R26" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="S26" s="76"/>
-      <c r="T26" s="76"/>
+      <c r="S26" s="134"/>
+      <c r="T26" s="134"/>
       <c r="U26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="V26" s="76"/>
-      <c r="W26" s="77"/>
+      <c r="V26" s="134"/>
+      <c r="W26" s="136"/>
     </row>
     <row r="27" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="98"/>
-      <c r="B27" s="99"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="30"/>
-      <c r="D27" s="73" t="str">
-        <f t="shared" ref="D27" si="7">IF(I27&lt;&gt;"",I27+J28,"")</f>
-        <v/>
-      </c>
-      <c r="E27" s="75"/>
+      <c r="D27" s="108" t="str">
+        <f>IF(I27&lt;&gt;"",MOD(I27+J28,360),"")</f>
+        <v/>
+      </c>
+      <c r="E27" s="110"/>
       <c r="F27" s="35"/>
       <c r="G27" s="32"/>
-      <c r="H27" s="57"/>
+      <c r="H27" s="90"/>
       <c r="I27" s="32"/>
       <c r="J27" s="47" t="str">
-        <f>IF(I27&lt;&gt;"",IF(ISNUMBER(I28),I27+I28,I27),"")</f>
+        <f>IF(I27&lt;&gt;"",IF(ISNUMBER(I28),MOD(I27+I28,360),I27),"")</f>
         <v/>
       </c>
       <c r="K27" s="47" t="str">
-        <f>IF(J27&lt;&gt;"",J27+J28,"")</f>
-        <v/>
-      </c>
-      <c r="L27" s="61" t="str">
-        <f t="shared" ref="L27" si="8">IF(K27&lt;&gt;"",K27+K28,"")</f>
+        <f>IF(J27&lt;&gt;"",MOD(J27+J28,360),"")</f>
+        <v/>
+      </c>
+      <c r="L27" s="128" t="str">
+        <f>IF(K27&lt;&gt;"",MOD(K27+K28,360),"")</f>
         <v/>
       </c>
       <c r="M27" s="35"/>
@@ -2898,30 +2891,30 @@
       <c r="R27" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="S27" s="76"/>
-      <c r="T27" s="76"/>
+      <c r="S27" s="134"/>
+      <c r="T27" s="134"/>
       <c r="U27" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="V27" s="76"/>
-      <c r="W27" s="77"/>
+      <c r="V27" s="134"/>
+      <c r="W27" s="136"/>
     </row>
-    <row r="28" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="98"/>
-      <c r="B28" s="99"/>
+    <row r="28" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="71"/>
+      <c r="B28" s="64"/>
       <c r="C28" s="30"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="102"/>
-      <c r="H28" s="58"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="91"/>
       <c r="I28" s="47" t="str">
         <f>IF(F27&lt;&gt;"",DEGREES(ASIN(G27/H27*SIN(RADIANS(F27-I27)))),"")</f>
         <v/>
       </c>
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
-      <c r="L28" s="60"/>
+      <c r="L28" s="129"/>
       <c r="M28" s="44" t="str">
         <f>IF(ISNUMBER(M27),M26-M27,"")</f>
         <v/>
@@ -2936,37 +2929,37 @@
       <c r="R28" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="S28" s="76"/>
-      <c r="T28" s="76"/>
+      <c r="S28" s="134"/>
+      <c r="T28" s="134"/>
       <c r="U28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="V28" s="76"/>
-      <c r="W28" s="77"/>
+      <c r="V28" s="134"/>
+      <c r="W28" s="136"/>
     </row>
     <row r="29" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="98"/>
-      <c r="B29" s="99"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="64"/>
       <c r="C29" s="30"/>
-      <c r="D29" s="73" t="str">
-        <f t="shared" ref="D29" si="9">IF(I29&lt;&gt;"",I29+J30,"")</f>
-        <v/>
-      </c>
-      <c r="E29" s="75"/>
+      <c r="D29" s="108" t="str">
+        <f>IF(I29&lt;&gt;"",MOD(I29+J30,360),"")</f>
+        <v/>
+      </c>
+      <c r="E29" s="110"/>
       <c r="F29" s="35"/>
       <c r="G29" s="32"/>
-      <c r="H29" s="57"/>
+      <c r="H29" s="90"/>
       <c r="I29" s="32"/>
       <c r="J29" s="47" t="str">
-        <f>IF(I29&lt;&gt;"",IF(ISNUMBER(I30),I29+I30,I29),"")</f>
+        <f>IF(I29&lt;&gt;"",IF(ISNUMBER(I30),MOD(I29+I30,360),I29),"")</f>
         <v/>
       </c>
       <c r="K29" s="47" t="str">
-        <f>IF(J29&lt;&gt;"",J29+J30,"")</f>
-        <v/>
-      </c>
-      <c r="L29" s="61" t="str">
-        <f t="shared" ref="L29" si="10">IF(K29&lt;&gt;"",K29+K30,"")</f>
+        <f>IF(J29&lt;&gt;"",MOD(J29+J30,360),"")</f>
+        <v/>
+      </c>
+      <c r="L29" s="128" t="str">
+        <f>IF(K29&lt;&gt;"",MOD(K29+K30,360),"")</f>
         <v/>
       </c>
       <c r="M29" s="35"/>
@@ -2986,30 +2979,30 @@
       <c r="R29" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="S29" s="76"/>
-      <c r="T29" s="76"/>
+      <c r="S29" s="134"/>
+      <c r="T29" s="134"/>
       <c r="U29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="V29" s="76"/>
-      <c r="W29" s="77"/>
+      <c r="V29" s="134"/>
+      <c r="W29" s="136"/>
     </row>
-    <row r="30" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="98"/>
-      <c r="B30" s="99"/>
+    <row r="30" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="71"/>
+      <c r="B30" s="64"/>
       <c r="C30" s="30"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="102"/>
-      <c r="H30" s="58"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="99"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="91"/>
       <c r="I30" s="47" t="str">
         <f>IF(F29&lt;&gt;"",DEGREES(ASIN(G29/H29*SIN(RADIANS(F29-I29)))),"")</f>
         <v/>
       </c>
       <c r="J30" s="32"/>
       <c r="K30" s="32"/>
-      <c r="L30" s="60"/>
+      <c r="L30" s="129"/>
       <c r="M30" s="44" t="str">
         <f>IF(ISNUMBER(M29),M28-M29,"")</f>
         <v/>
@@ -3024,37 +3017,37 @@
       <c r="R30" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="S30" s="76"/>
-      <c r="T30" s="76"/>
+      <c r="S30" s="134"/>
+      <c r="T30" s="134"/>
       <c r="U30" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="V30" s="76"/>
-      <c r="W30" s="77"/>
+      <c r="V30" s="134"/>
+      <c r="W30" s="136"/>
     </row>
     <row r="31" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="98"/>
-      <c r="B31" s="99"/>
+      <c r="A31" s="71"/>
+      <c r="B31" s="64"/>
       <c r="C31" s="30"/>
-      <c r="D31" s="73" t="str">
-        <f t="shared" ref="D31" si="11">IF(I31&lt;&gt;"",I31+J32,"")</f>
-        <v/>
-      </c>
-      <c r="E31" s="75"/>
+      <c r="D31" s="108" t="str">
+        <f>IF(I31&lt;&gt;"",MOD(I31+J32,360),"")</f>
+        <v/>
+      </c>
+      <c r="E31" s="110"/>
       <c r="F31" s="35"/>
       <c r="G31" s="32"/>
-      <c r="H31" s="65"/>
+      <c r="H31" s="132"/>
       <c r="I31" s="32"/>
       <c r="J31" s="47" t="str">
-        <f>IF(I31&lt;&gt;"",IF(ISNUMBER(I32),I31+I32,I31),"")</f>
+        <f>IF(I31&lt;&gt;"",IF(ISNUMBER(I32),MOD(I31+I32,360),I31),"")</f>
         <v/>
       </c>
       <c r="K31" s="47" t="str">
-        <f>IF(J31&lt;&gt;"",J31+J32,"")</f>
-        <v/>
-      </c>
-      <c r="L31" s="61" t="str">
-        <f>IF(K31&lt;&gt;"",K31+K32,"")</f>
+        <f>IF(J31&lt;&gt;"",MOD(J31+J32,360),"")</f>
+        <v/>
+      </c>
+      <c r="L31" s="128" t="str">
+        <f>IF(K31&lt;&gt;"",MOD(K31+K32,360),"")</f>
         <v/>
       </c>
       <c r="M31" s="35"/>
@@ -3074,27 +3067,27 @@
       <c r="R31" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="S31" s="78"/>
-      <c r="T31" s="78"/>
+      <c r="S31" s="135"/>
+      <c r="T31" s="135"/>
       <c r="U31" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="V31" s="78"/>
-      <c r="W31" s="79"/>
+      <c r="V31" s="135"/>
+      <c r="W31" s="137"/>
     </row>
     <row r="32" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="98"/>
-      <c r="B32" s="99"/>
+      <c r="A32" s="71"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="30"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="112"/>
-      <c r="H32" s="66"/>
+      <c r="D32" s="109"/>
+      <c r="E32" s="124"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="133"/>
       <c r="I32" s="48"/>
       <c r="J32" s="33"/>
       <c r="K32" s="33"/>
-      <c r="L32" s="62"/>
+      <c r="L32" s="129"/>
       <c r="M32" s="44" t="str">
         <f>IF(ISNUMBER(M31),M30-M31,"")</f>
         <v/>
@@ -3106,32 +3099,32 @@
         <f>IF(AND(ISNUMBER(Q30),ISNUMBER(Q31)),Q30-Q31,"")</f>
         <v/>
       </c>
-      <c r="R32" s="67" t="s">
+      <c r="R32" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="S32" s="68"/>
-      <c r="T32" s="90"/>
-      <c r="U32" s="90"/>
-      <c r="V32" s="90" t="s">
+      <c r="S32" s="121"/>
+      <c r="T32" s="95"/>
+      <c r="U32" s="95"/>
+      <c r="V32" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="W32" s="113"/>
+      <c r="W32" s="96"/>
     </row>
     <row r="33" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="114"/>
-      <c r="B33" s="89"/>
+      <c r="A33" s="80"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="23"/>
-      <c r="D33" s="71" t="s">
+      <c r="D33" s="122" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="72"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="122"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="123"/>
       <c r="M33" s="24">
         <f>SUM(M13,M15,M17,M19,M21,M23,M25,M27,M29,M31)</f>
         <v>0</v>
@@ -3146,14 +3139,14 @@
         <f>SUM(Q13,Q15,Q17,Q19,Q21,Q23,Q25,Q27,Q29,Q31)</f>
         <v>0</v>
       </c>
-      <c r="R33" s="69" t="s">
+      <c r="R33" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="S33" s="70"/>
-      <c r="T33" s="88"/>
-      <c r="U33" s="88"/>
-      <c r="V33" s="88"/>
-      <c r="W33" s="89"/>
+      <c r="S33" s="75"/>
+      <c r="T33" s="61"/>
+      <c r="U33" s="61"/>
+      <c r="V33" s="61"/>
+      <c r="W33" s="65"/>
     </row>
     <row r="34" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
@@ -3219,46 +3212,96 @@
     </row>
   </sheetData>
   <mergeCells count="156">
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N2:W8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="A9:B11"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="D33:L33"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="R21:W21"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="T12:U12"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="G1:P1"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="H13:H14"/>
     <mergeCell ref="T16:U16"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="F32:G32"/>
@@ -3283,97 +3326,47 @@
     <mergeCell ref="A24:B25"/>
     <mergeCell ref="A26:B27"/>
     <mergeCell ref="A14:B15"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="G1:P1"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="D33:L33"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="R21:W21"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N2:W8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="L29:L30"/>
     <mergeCell ref="J3:M3"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>

<commit_message>
Use lighter color shades for formatting
Lighter color shades make it easy to read a color printed hard copy
</commit_message>
<xml_diff>
--- a/vaayuyaana/jagiNavLog.xlsx
+++ b/vaayuyaana/jagiNavLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hanchu\code\github.com\jkanasu\utilities\vaayuyaana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F5A7AF-6D42-4954-9E8C-623D44FF5F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778DC308-82AC-4B0E-A337-F2B3219C6E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3DE2A8C-E23C-4F63-95E8-9AD5B4E402C0}"/>
   </bookViews>
@@ -492,19 +492,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,7 +1292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1315,30 +1315,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1354,12 +1330,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1369,34 +1339,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1405,493 +1351,541 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1901,6 +1895,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2291,7 +2291,7 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,1448 +2310,1448 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="184" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="184"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="138" t="s">
+      <c r="H1" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="138"/>
-      <c r="Q1" s="138"/>
-      <c r="R1" s="63" t="s">
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="64"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="66"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="38"/>
     </row>
     <row r="2" spans="1:24" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="62" t="s">
+      <c r="B2" s="130"/>
+      <c r="C2" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="62" t="s">
+      <c r="D2" s="130"/>
+      <c r="E2" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="125"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="62" t="s">
+      <c r="F2" s="131"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="123"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="49" t="s">
+      <c r="I2" s="133"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="47"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="116"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="106"/>
     </row>
     <row r="3" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="185"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="187"/>
-      <c r="D3" s="144" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="145"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="73" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="97" t="s">
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="144"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118"/>
-      <c r="V3" s="118"/>
-      <c r="W3" s="118"/>
-      <c r="X3" s="119"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="107"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="109"/>
     </row>
     <row r="4" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="131"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="179"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="172" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="173"/>
-      <c r="M4" s="126"/>
-      <c r="N4" s="127"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="118"/>
-      <c r="Q4" s="118"/>
-      <c r="R4" s="118"/>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="118"/>
-      <c r="X4" s="119"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="163"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="107"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="108"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="108"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="108"/>
+      <c r="W4" s="108"/>
+      <c r="X4" s="109"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="178"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="140"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="172" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="138"/>
+      <c r="I5" s="138"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="173"/>
-      <c r="M5" s="126"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="118"/>
-      <c r="R5" s="118"/>
-      <c r="S5" s="118"/>
-      <c r="T5" s="118"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="118"/>
-      <c r="X5" s="119"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="164"/>
+      <c r="O5" s="107"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="109"/>
     </row>
     <row r="6" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="130" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="131"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="178"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="172" t="s">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="137"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="173"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="118"/>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
-      <c r="S6" s="118"/>
-      <c r="T6" s="118"/>
-      <c r="U6" s="118"/>
-      <c r="V6" s="118"/>
-      <c r="W6" s="118"/>
-      <c r="X6" s="119"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="163"/>
+      <c r="N6" s="164"/>
+      <c r="O6" s="107"/>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="108"/>
+      <c r="R6" s="108"/>
+      <c r="S6" s="108"/>
+      <c r="T6" s="108"/>
+      <c r="U6" s="108"/>
+      <c r="V6" s="108"/>
+      <c r="W6" s="108"/>
+      <c r="X6" s="109"/>
     </row>
     <row r="7" spans="1:24" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="131"/>
-      <c r="C7" s="131"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="179"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="172" t="s">
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="173"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="127"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="118"/>
-      <c r="Q7" s="118"/>
-      <c r="R7" s="118"/>
-      <c r="S7" s="118"/>
-      <c r="T7" s="118"/>
-      <c r="U7" s="118"/>
-      <c r="V7" s="118"/>
-      <c r="W7" s="118"/>
-      <c r="X7" s="119"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="163"/>
+      <c r="N7" s="164"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="108"/>
+      <c r="V7" s="108"/>
+      <c r="W7" s="108"/>
+      <c r="X7" s="109"/>
     </row>
     <row r="8" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132" t="s">
+      <c r="A8" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="191"/>
-      <c r="F8" s="167"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="174" t="s">
+      <c r="B8" s="114"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="140"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="143"/>
+      <c r="J8" s="144"/>
+      <c r="K8" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="175"/>
-      <c r="M8" s="128"/>
-      <c r="N8" s="129"/>
-      <c r="O8" s="120"/>
-      <c r="P8" s="121"/>
-      <c r="Q8" s="121"/>
-      <c r="R8" s="121"/>
-      <c r="S8" s="121"/>
-      <c r="T8" s="121"/>
-      <c r="U8" s="121"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="121"/>
-      <c r="X8" s="122"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="165"/>
+      <c r="N8" s="166"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
+      <c r="T8" s="111"/>
+      <c r="U8" s="111"/>
+      <c r="V8" s="111"/>
+      <c r="W8" s="111"/>
+      <c r="X8" s="112"/>
     </row>
     <row r="9" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="80"/>
+      <c r="C9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="101" t="s">
+      <c r="D9" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="104" t="s">
+      <c r="E9" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="111" t="s">
+      <c r="F9" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="97" t="s">
+      <c r="G9" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="73"/>
-      <c r="I9" s="38" t="s">
+      <c r="H9" s="79"/>
+      <c r="I9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="145" t="s">
+      <c r="M9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="73" t="s">
+      <c r="P9" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="20" t="s">
+      <c r="Q9" s="79"/>
+      <c r="R9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="S9" s="72" t="s">
+      <c r="S9" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="T9" s="73"/>
-      <c r="U9" s="76" t="s">
+      <c r="T9" s="79"/>
+      <c r="U9" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="V9" s="73"/>
-      <c r="W9" s="73" t="s">
+      <c r="V9" s="79"/>
+      <c r="W9" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="X9" s="77"/>
+      <c r="X9" s="80"/>
     </row>
     <row r="10" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99"/>
+      <c r="A10" s="90"/>
+      <c r="B10" s="91"/>
       <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="102"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="26" t="s">
+      <c r="D10" s="94"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="39" t="s">
+      <c r="I10" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="107" t="s">
+      <c r="J10" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="134" t="s">
+      <c r="K10" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="136" t="s">
+      <c r="L10" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="146"/>
-      <c r="N10" s="26" t="s">
+      <c r="M10" s="87"/>
+      <c r="N10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="25" t="s">
+      <c r="O10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="15" t="str">
+      <c r="P10" s="170"/>
+      <c r="Q10" s="170"/>
+      <c r="R10" s="153" t="str">
         <f>IF(ISNUMBER(J34),J34,"")</f>
         <v/>
       </c>
-      <c r="S10" s="74"/>
-      <c r="T10" s="75"/>
-      <c r="U10" s="75"/>
-      <c r="V10" s="75"/>
-      <c r="W10" s="75"/>
-      <c r="X10" s="78"/>
+      <c r="S10" s="77"/>
+      <c r="T10" s="78"/>
+      <c r="U10" s="78"/>
+      <c r="V10" s="78"/>
+      <c r="W10" s="78"/>
+      <c r="X10" s="83"/>
     </row>
     <row r="11" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="100"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="34" t="s">
+      <c r="A11" s="92"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="102"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="180" t="s">
+      <c r="D11" s="94"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="148"/>
-      <c r="I11" s="170" t="s">
+      <c r="H11" s="65"/>
+      <c r="I11" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="107"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="136"/>
-      <c r="M11" s="146"/>
-      <c r="N11" s="26" t="s">
+      <c r="J11" s="99"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="117"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="O11" s="148" t="s">
+      <c r="O11" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="P11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="Q11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="27" t="s">
+      <c r="R11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="S11" s="94"/>
-      <c r="T11" s="95"/>
-      <c r="U11" s="155" t="s">
+      <c r="S11" s="167"/>
+      <c r="T11" s="168"/>
+      <c r="U11" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="V11" s="155"/>
-      <c r="W11" s="95"/>
-      <c r="X11" s="152"/>
+      <c r="V11" s="84"/>
+      <c r="W11" s="168"/>
+      <c r="X11" s="173"/>
     </row>
     <row r="12" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="193" t="s">
+      <c r="A12" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="194"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="181"/>
-      <c r="H12" s="156"/>
-      <c r="I12" s="171"/>
-      <c r="J12" s="108"/>
-      <c r="K12" s="135"/>
-      <c r="L12" s="137"/>
-      <c r="M12" s="147"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="149"/>
-      <c r="P12" s="21" t="s">
+      <c r="D12" s="95"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="103"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="118"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="160"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Q12" s="21" t="s">
+      <c r="Q12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="R12" s="22" t="s">
+      <c r="R12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="S12" s="96"/>
-      <c r="T12" s="82"/>
-      <c r="U12" s="148" t="s">
+      <c r="S12" s="169"/>
+      <c r="T12" s="170"/>
+      <c r="U12" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="V12" s="148"/>
-      <c r="W12" s="82"/>
-      <c r="X12" s="153"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="170"/>
+      <c r="X12" s="174"/>
     </row>
     <row r="13" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="195"/>
-      <c r="B13" s="196"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="139" t="str">
+      <c r="A13" s="43"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="184" t="str">
         <f>IF(J13&lt;&gt;"",MOD(J13+K14,360),"")</f>
         <v/>
       </c>
-      <c r="E13" s="168"/>
-      <c r="F13" s="201" t="str">
+      <c r="E13" s="145"/>
+      <c r="F13" s="186" t="str">
         <f>IF(ISNUMBER(E13),15-E13/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="37" t="str">
+      <c r="G13" s="146"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="146"/>
+      <c r="K13" s="190" t="str">
         <f>IF(J13&lt;&gt;"",IF(ISNUMBER(J14),MOD(J13+J14,360),J13),"")</f>
         <v/>
       </c>
-      <c r="L13" s="40" t="str">
+      <c r="L13" s="191" t="str">
         <f>IF(K13&lt;&gt;"",MOD(K13+K14,360),"")</f>
         <v/>
       </c>
-      <c r="M13" s="142" t="str">
+      <c r="M13" s="192" t="str">
         <f>IF(L13&lt;&gt;"",MOD(L13+L14,360),"")</f>
         <v/>
       </c>
-      <c r="N13" s="14" t="str">
+      <c r="N13" s="189" t="str">
         <f>IF(AND(ISNUMBER(O13),ISNUMBER(P13)),ROUND(P13*O13/60,0),"")</f>
         <v/>
       </c>
-      <c r="O13" s="13" t="str">
+      <c r="O13" s="198" t="str">
         <f>IF(ISNUMBER(I13),SQRT((H13^2) + (I13^2) - (2*H13*I13*COS(   ACOS(COS(RADIANS(J13-G13)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="24" t="str">
+      <c r="P13" s="161"/>
+      <c r="Q13" s="180"/>
+      <c r="R13" s="162" t="str">
         <f>IF(ISNUMBER(P13),P13*$R$10/60,"")</f>
         <v/>
       </c>
-      <c r="S13" s="96"/>
-      <c r="T13" s="82"/>
-      <c r="U13" s="148" t="s">
+      <c r="S13" s="169"/>
+      <c r="T13" s="170"/>
+      <c r="U13" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="V13" s="148"/>
-      <c r="W13" s="82"/>
-      <c r="X13" s="153"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="170"/>
+      <c r="X13" s="174"/>
     </row>
     <row r="14" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="197" t="s">
+      <c r="A14" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="198"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="139"/>
-      <c r="E14" s="140"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="14" t="str">
+      <c r="B14" s="46"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="184"/>
+      <c r="E14" s="137"/>
+      <c r="F14" s="187"/>
+      <c r="G14" s="149"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="189" t="str">
         <f>IF(G13&lt;&gt;"",DEGREES(ASIN(H13/I13*SIN(RADIANS(G13-J13)))),"")</f>
         <v/>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="143"/>
-      <c r="N14" s="14" t="str">
+      <c r="K14" s="151"/>
+      <c r="L14" s="153"/>
+      <c r="M14" s="193"/>
+      <c r="N14" s="189" t="str">
         <f>IF(ISNUMBER(N13),N12-N13,"")</f>
         <v/>
       </c>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="11" t="str">
+      <c r="O14" s="181"/>
+      <c r="P14" s="181"/>
+      <c r="Q14" s="181"/>
+      <c r="R14" s="197" t="str">
         <f>IF(AND(ISNUMBER(R34),ISNUMBER(R13)),R34-$M$34-R13,"")</f>
         <v/>
       </c>
-      <c r="S14" s="96"/>
-      <c r="T14" s="82"/>
-      <c r="U14" s="148" t="s">
+      <c r="S14" s="169"/>
+      <c r="T14" s="170"/>
+      <c r="U14" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="V14" s="148"/>
-      <c r="W14" s="82"/>
-      <c r="X14" s="153"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="170"/>
+      <c r="X14" s="174"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="195"/>
-      <c r="B15" s="196"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="139" t="str">
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="184" t="str">
         <f>IF(J15&lt;&gt;"",MOD(J15+K16,360),"")</f>
         <v/>
       </c>
-      <c r="E15" s="140"/>
-      <c r="F15" s="201" t="str">
+      <c r="E15" s="137"/>
+      <c r="F15" s="186" t="str">
         <f t="shared" ref="F15" si="0">IF(ISNUMBER(E15),15-E15/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="12" t="str">
+      <c r="G15" s="150"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="150"/>
+      <c r="K15" s="196" t="str">
         <f>IF(J15&lt;&gt;"",IF(ISNUMBER(J16),MOD(J15+J16,360),J15),"")</f>
         <v/>
       </c>
-      <c r="L15" s="11" t="str">
+      <c r="L15" s="197" t="str">
         <f>IF(K15&lt;&gt;"",MOD(K15+K16,360),"")</f>
         <v/>
       </c>
-      <c r="M15" s="143" t="str">
+      <c r="M15" s="193" t="str">
         <f>IF(L15&lt;&gt;"",MOD(L15+L16,360),"")</f>
         <v/>
       </c>
-      <c r="N15" s="28"/>
-      <c r="O15" s="12" t="str">
+      <c r="N15" s="150"/>
+      <c r="O15" s="196" t="str">
         <f>IF(ISNUMBER(I15),SQRT((H15^2) + (I15^2) - (2*H15*I15*COS(   ACOS(COS(RADIANS(J15-G15)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P15" s="12" t="str">
+      <c r="P15" s="196" t="str">
         <f>IF(ISNUMBER(O15),ROUND(N15/O15*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="15" t="str">
+      <c r="Q15" s="181"/>
+      <c r="R15" s="153" t="str">
         <f>IF(ISNUMBER(P15),P15*$R$10/60,"")</f>
         <v/>
       </c>
-      <c r="S15" s="96"/>
-      <c r="T15" s="82"/>
-      <c r="U15" s="148" t="s">
+      <c r="S15" s="169"/>
+      <c r="T15" s="170"/>
+      <c r="U15" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="V15" s="148"/>
-      <c r="W15" s="82"/>
-      <c r="X15" s="153"/>
+      <c r="V15" s="65"/>
+      <c r="W15" s="170"/>
+      <c r="X15" s="174"/>
     </row>
     <row r="16" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="197"/>
-      <c r="B16" s="198"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="139"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="14" t="str">
+      <c r="A16" s="45"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="184"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="187"/>
+      <c r="G16" s="149"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="189" t="str">
         <f>IF(G15&lt;&gt;"",DEGREES(ASIN(H15/I15*SIN(RADIANS(G15-J15)))),"")</f>
         <v/>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="143"/>
-      <c r="N16" s="14" t="str">
+      <c r="K16" s="151"/>
+      <c r="L16" s="153"/>
+      <c r="M16" s="193"/>
+      <c r="N16" s="189" t="str">
         <f>IF(ISNUMBER(N15),N14-N15,"")</f>
         <v/>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="11" t="str">
+      <c r="O16" s="181"/>
+      <c r="P16" s="181"/>
+      <c r="Q16" s="181"/>
+      <c r="R16" s="197" t="str">
         <f>IF(AND(ISNUMBER(R14),ISNUMBER(R15)),R14-R15,"")</f>
         <v/>
       </c>
-      <c r="S16" s="96"/>
-      <c r="T16" s="82"/>
-      <c r="U16" s="148" t="s">
+      <c r="S16" s="169"/>
+      <c r="T16" s="170"/>
+      <c r="U16" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="V16" s="148"/>
-      <c r="W16" s="82"/>
-      <c r="X16" s="153"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="170"/>
+      <c r="X16" s="174"/>
     </row>
     <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="195"/>
-      <c r="B17" s="196"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="139" t="str">
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="184" t="str">
         <f>IF(J17&lt;&gt;"",MOD(J17+K18,360),"")</f>
         <v/>
       </c>
-      <c r="E17" s="140"/>
-      <c r="F17" s="201" t="str">
+      <c r="E17" s="137"/>
+      <c r="F17" s="186" t="str">
         <f t="shared" ref="F17" si="1">IF(ISNUMBER(E17),15-E17/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="12" t="str">
+      <c r="G17" s="150"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="150"/>
+      <c r="K17" s="196" t="str">
         <f>IF(J17&lt;&gt;"",IF(ISNUMBER(J18),MOD(J17+J18,360),J17),"")</f>
         <v/>
       </c>
-      <c r="L17" s="11" t="str">
+      <c r="L17" s="197" t="str">
         <f>IF(K17&lt;&gt;"",MOD(K17+K18,360),"")</f>
         <v/>
       </c>
-      <c r="M17" s="143" t="str">
+      <c r="M17" s="193" t="str">
         <f>IF(L17&lt;&gt;"",MOD(L17+L18,360),"")</f>
         <v/>
       </c>
-      <c r="N17" s="28"/>
-      <c r="O17" s="12" t="str">
+      <c r="N17" s="150"/>
+      <c r="O17" s="196" t="str">
         <f>IF(ISNUMBER(I17),SQRT((H17^2) + (I17^2) - (2*H17*I17*COS(   ACOS(COS(RADIANS(J17-G17)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P17" s="12" t="str">
+      <c r="P17" s="196" t="str">
         <f>IF(ISNUMBER(O17),ROUND(N17/O17*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="15" t="str">
+      <c r="Q17" s="181"/>
+      <c r="R17" s="153" t="str">
         <f>IF(ISNUMBER(P17),P17*$R$10/60,"")</f>
         <v/>
       </c>
-      <c r="S17" s="150"/>
-      <c r="T17" s="151"/>
-      <c r="U17" s="156" t="s">
+      <c r="S17" s="171"/>
+      <c r="T17" s="172"/>
+      <c r="U17" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="V17" s="156"/>
-      <c r="W17" s="151"/>
-      <c r="X17" s="164"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="172"/>
+      <c r="X17" s="175"/>
     </row>
     <row r="18" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="197"/>
-      <c r="B18" s="198"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="139"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="176"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="14" t="str">
+      <c r="D18" s="184"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="187"/>
+      <c r="G18" s="149"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="139"/>
+      <c r="J18" s="189" t="str">
         <f>IF(G17&lt;&gt;"",DEGREES(ASIN(H17/I17*SIN(RADIANS(G17-J17)))),"")</f>
         <v/>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="14" t="str">
+      <c r="K18" s="151"/>
+      <c r="L18" s="153"/>
+      <c r="M18" s="193"/>
+      <c r="N18" s="189" t="str">
         <f>IF(ISNUMBER(N17),N16-N17,"")</f>
         <v/>
       </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="11" t="str">
+      <c r="O18" s="181"/>
+      <c r="P18" s="181"/>
+      <c r="Q18" s="181"/>
+      <c r="R18" s="197" t="str">
         <f>IF(AND(ISNUMBER(R16),ISNUMBER(R17)),R16-R17,"")</f>
         <v/>
       </c>
-      <c r="S18" s="83"/>
-      <c r="T18" s="84"/>
-      <c r="U18" s="84"/>
-      <c r="V18" s="84"/>
-      <c r="W18" s="84"/>
-      <c r="X18" s="85"/>
+      <c r="S18" s="121"/>
+      <c r="T18" s="122"/>
+      <c r="U18" s="122"/>
+      <c r="V18" s="122"/>
+      <c r="W18" s="122"/>
+      <c r="X18" s="123"/>
     </row>
     <row r="19" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="195"/>
-      <c r="B19" s="196"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="139" t="str">
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="184" t="str">
         <f>IF(J19&lt;&gt;"",MOD(J19+K20,360),"")</f>
         <v/>
       </c>
-      <c r="E19" s="140"/>
-      <c r="F19" s="201" t="str">
+      <c r="E19" s="137"/>
+      <c r="F19" s="186" t="str">
         <f t="shared" ref="F19" si="2">IF(ISNUMBER(E19),15-E19/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="12" t="str">
+      <c r="G19" s="150"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="139"/>
+      <c r="J19" s="150"/>
+      <c r="K19" s="196" t="str">
         <f>IF(J19&lt;&gt;"",IF(ISNUMBER(J20),MOD(J19+J20,360),J19),"")</f>
         <v/>
       </c>
-      <c r="L19" s="11" t="str">
+      <c r="L19" s="197" t="str">
         <f>IF(K19&lt;&gt;"",MOD(K19+K20,360),"")</f>
         <v/>
       </c>
-      <c r="M19" s="143" t="str">
+      <c r="M19" s="193" t="str">
         <f>IF(L19&lt;&gt;"",MOD(L19+L20,360),"")</f>
         <v/>
       </c>
-      <c r="N19" s="28"/>
-      <c r="O19" s="12" t="str">
+      <c r="N19" s="150"/>
+      <c r="O19" s="196" t="str">
         <f>IF(ISNUMBER(I19),SQRT((H19^2) + (I19^2) - (2*H19*I19*COS(   ACOS(COS(RADIANS(J19-G19)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P19" s="12" t="str">
+      <c r="P19" s="196" t="str">
         <f>IF(ISNUMBER(O19),ROUND(N19/O19*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="15" t="str">
+      <c r="Q19" s="181"/>
+      <c r="R19" s="153" t="str">
         <f>IF(ISNUMBER(P19),P19*$R$10/60,"")</f>
         <v/>
       </c>
-      <c r="S19" s="86"/>
-      <c r="T19" s="87"/>
-      <c r="U19" s="87"/>
-      <c r="V19" s="87"/>
-      <c r="W19" s="87"/>
-      <c r="X19" s="88"/>
+      <c r="S19" s="124"/>
+      <c r="T19" s="125"/>
+      <c r="U19" s="125"/>
+      <c r="V19" s="125"/>
+      <c r="W19" s="125"/>
+      <c r="X19" s="126"/>
     </row>
     <row r="20" spans="1:24" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="197"/>
-      <c r="B20" s="198"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="139"/>
-      <c r="E20" s="140"/>
-      <c r="F20" s="176"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="14" t="str">
+      <c r="D20" s="184"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="187"/>
+      <c r="G20" s="149"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="139"/>
+      <c r="J20" s="189" t="str">
         <f>IF(G19&lt;&gt;"",DEGREES(ASIN(H19/I19*SIN(RADIANS(G19-J19)))),"")</f>
         <v/>
       </c>
-      <c r="K20" s="29"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="143"/>
-      <c r="N20" s="14" t="str">
+      <c r="K20" s="151"/>
+      <c r="L20" s="153"/>
+      <c r="M20" s="193"/>
+      <c r="N20" s="189" t="str">
         <f>IF(ISNUMBER(N19),N18-N19,"")</f>
         <v/>
       </c>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="11" t="str">
+      <c r="O20" s="181"/>
+      <c r="P20" s="181"/>
+      <c r="Q20" s="181"/>
+      <c r="R20" s="197" t="str">
         <f>IF(AND(ISNUMBER(R18),ISNUMBER(R19)),R18-R19,"")</f>
         <v/>
       </c>
-      <c r="S20" s="89"/>
-      <c r="T20" s="90"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="90"/>
-      <c r="W20" s="90"/>
-      <c r="X20" s="91"/>
+      <c r="S20" s="127"/>
+      <c r="T20" s="128"/>
+      <c r="U20" s="128"/>
+      <c r="V20" s="128"/>
+      <c r="W20" s="128"/>
+      <c r="X20" s="129"/>
     </row>
     <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="195"/>
-      <c r="B21" s="196"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="139" t="str">
+      <c r="A21" s="43"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="184" t="str">
         <f>IF(J21&lt;&gt;"",MOD(J21+K22,360),"")</f>
         <v/>
       </c>
-      <c r="E21" s="140"/>
-      <c r="F21" s="201" t="str">
+      <c r="E21" s="137"/>
+      <c r="F21" s="186" t="str">
         <f t="shared" ref="F21" si="3">IF(ISNUMBER(E21),15-E21/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="12" t="str">
+      <c r="G21" s="150"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="139"/>
+      <c r="J21" s="150"/>
+      <c r="K21" s="196" t="str">
         <f>IF(J21&lt;&gt;"",IF(ISNUMBER(J22),MOD(J21+J22,360),J21),"")</f>
         <v/>
       </c>
-      <c r="L21" s="11" t="str">
+      <c r="L21" s="197" t="str">
         <f>IF(K21&lt;&gt;"",MOD(K21+K22,360),"")</f>
         <v/>
       </c>
-      <c r="M21" s="143" t="str">
+      <c r="M21" s="193" t="str">
         <f>IF(L21&lt;&gt;"",MOD(L21+L22,360),"")</f>
         <v/>
       </c>
-      <c r="N21" s="28"/>
-      <c r="O21" s="12" t="str">
+      <c r="N21" s="150"/>
+      <c r="O21" s="196" t="str">
         <f>IF(ISNUMBER(I21),SQRT((H21^2) + (I21^2) - (2*H21*I21*COS(   ACOS(COS(RADIANS(J21-G21)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P21" s="12" t="str">
+      <c r="P21" s="196" t="str">
         <f>IF(ISNUMBER(O21),ROUND(N21/O21*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="15" t="str">
+      <c r="Q21" s="181"/>
+      <c r="R21" s="153" t="str">
         <f>IF(ISNUMBER(P21),P21*$R$10/60,"")</f>
         <v/>
       </c>
-      <c r="S21" s="72" t="s">
+      <c r="S21" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="T21" s="73"/>
-      <c r="U21" s="73"/>
-      <c r="V21" s="73"/>
-      <c r="W21" s="73"/>
-      <c r="X21" s="77"/>
+      <c r="T21" s="79"/>
+      <c r="U21" s="79"/>
+      <c r="V21" s="79"/>
+      <c r="W21" s="79"/>
+      <c r="X21" s="80"/>
     </row>
     <row r="22" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="197"/>
-      <c r="B22" s="198"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="139"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="176"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="80"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="14" t="str">
+      <c r="D22" s="184"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="187"/>
+      <c r="G22" s="149"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="139"/>
+      <c r="J22" s="189" t="str">
         <f>IF(G21&lt;&gt;"",DEGREES(ASIN(H21/I21*SIN(RADIANS(G21-J21)))),"")</f>
         <v/>
       </c>
-      <c r="K22" s="29"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="143"/>
-      <c r="N22" s="14" t="str">
+      <c r="K22" s="151"/>
+      <c r="L22" s="153"/>
+      <c r="M22" s="193"/>
+      <c r="N22" s="189" t="str">
         <f>IF(ISNUMBER(N21),N20-N21,"")</f>
         <v/>
       </c>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="11" t="str">
+      <c r="O22" s="181"/>
+      <c r="P22" s="181"/>
+      <c r="Q22" s="181"/>
+      <c r="R22" s="197" t="str">
         <f>IF(AND(ISNUMBER(R20),ISNUMBER(R21)),R20-R21,"")</f>
         <v/>
       </c>
-      <c r="S22" s="74" t="s">
+      <c r="S22" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="T22" s="75"/>
-      <c r="U22" s="75"/>
-      <c r="V22" s="75" t="s">
+      <c r="T22" s="78"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="W22" s="75"/>
-      <c r="X22" s="78"/>
+      <c r="W22" s="78"/>
+      <c r="X22" s="83"/>
     </row>
     <row r="23" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="195"/>
-      <c r="B23" s="196"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="139" t="str">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="184" t="str">
         <f>IF(J23&lt;&gt;"",MOD(J23+K24,360),"")</f>
         <v/>
       </c>
-      <c r="E23" s="140"/>
-      <c r="F23" s="201" t="str">
+      <c r="E23" s="137"/>
+      <c r="F23" s="186" t="str">
         <f t="shared" ref="F23" si="4">IF(ISNUMBER(E23),15-E23/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="12" t="str">
+      <c r="G23" s="150"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="139"/>
+      <c r="J23" s="150"/>
+      <c r="K23" s="196" t="str">
         <f>IF(J23&lt;&gt;"",IF(ISNUMBER(J24),MOD(J23+J24,360),J23),"")</f>
         <v/>
       </c>
-      <c r="L23" s="11" t="str">
+      <c r="L23" s="197" t="str">
         <f>IF(K23&lt;&gt;"",MOD(K23+K24,360),"")</f>
         <v/>
       </c>
-      <c r="M23" s="143" t="str">
+      <c r="M23" s="193" t="str">
         <f>IF(L23&lt;&gt;"",MOD(L23+L24,360),"")</f>
         <v/>
       </c>
-      <c r="N23" s="28"/>
-      <c r="O23" s="12" t="str">
+      <c r="N23" s="150"/>
+      <c r="O23" s="196" t="str">
         <f>IF(ISNUMBER(I23),SQRT((H23^2) + (I23^2) - (2*H23*I23*COS(   ACOS(COS(RADIANS(J23-G23)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P23" s="12" t="str">
+      <c r="P23" s="196" t="str">
         <f>IF(ISNUMBER(O23),ROUND(N23/O23*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="15" t="str">
+      <c r="Q23" s="181"/>
+      <c r="R23" s="153" t="str">
         <f>IF(ISNUMBER(P23),P23*$R$10/60,"")</f>
         <v/>
       </c>
-      <c r="S23" s="94"/>
-      <c r="T23" s="95"/>
-      <c r="U23" s="95"/>
-      <c r="V23" s="95"/>
-      <c r="W23" s="95"/>
-      <c r="X23" s="152"/>
+      <c r="S23" s="167"/>
+      <c r="T23" s="168"/>
+      <c r="U23" s="168"/>
+      <c r="V23" s="168"/>
+      <c r="W23" s="168"/>
+      <c r="X23" s="173"/>
     </row>
     <row r="24" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="197"/>
-      <c r="B24" s="198"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="139"/>
-      <c r="E24" s="140"/>
-      <c r="F24" s="176"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="81"/>
-      <c r="J24" s="14" t="str">
+      <c r="A24" s="45"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="184"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="187"/>
+      <c r="G24" s="149"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="139"/>
+      <c r="J24" s="189" t="str">
         <f>IF(G23&lt;&gt;"",DEGREES(ASIN(H23/I23*SIN(RADIANS(G23-J23)))),"")</f>
         <v/>
       </c>
-      <c r="K24" s="29"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="143"/>
-      <c r="N24" s="14" t="str">
+      <c r="K24" s="151"/>
+      <c r="L24" s="153"/>
+      <c r="M24" s="193"/>
+      <c r="N24" s="189" t="str">
         <f>IF(ISNUMBER(N23),N22-N23,"")</f>
         <v/>
       </c>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="11" t="str">
+      <c r="O24" s="181"/>
+      <c r="P24" s="181"/>
+      <c r="Q24" s="181"/>
+      <c r="R24" s="197" t="str">
         <f>IF(AND(ISNUMBER(R22),ISNUMBER(R23)),R22-R23,"")</f>
         <v/>
       </c>
       <c r="S24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T24" s="71"/>
-      <c r="U24" s="71"/>
+      <c r="T24" s="176"/>
+      <c r="U24" s="176"/>
       <c r="V24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W24" s="71"/>
-      <c r="X24" s="154"/>
+      <c r="W24" s="176"/>
+      <c r="X24" s="177"/>
     </row>
     <row r="25" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="195"/>
-      <c r="B25" s="196"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="139" t="str">
+      <c r="A25" s="43"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="184" t="str">
         <f>IF(J25&lt;&gt;"",MOD(J25+K26,360),"")</f>
         <v/>
       </c>
-      <c r="E25" s="140"/>
-      <c r="F25" s="201" t="str">
+      <c r="E25" s="137"/>
+      <c r="F25" s="186" t="str">
         <f t="shared" ref="F25" si="5">IF(ISNUMBER(E25),15-E25/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="81"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="12" t="str">
+      <c r="G25" s="150"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="139"/>
+      <c r="J25" s="150"/>
+      <c r="K25" s="196" t="str">
         <f>IF(J25&lt;&gt;"",IF(ISNUMBER(J26),MOD(J25+J26,360),J25),"")</f>
         <v/>
       </c>
-      <c r="L25" s="11" t="str">
+      <c r="L25" s="197" t="str">
         <f>IF(K25&lt;&gt;"",MOD(K25+K26,360),"")</f>
         <v/>
       </c>
-      <c r="M25" s="143" t="str">
+      <c r="M25" s="193" t="str">
         <f>IF(L25&lt;&gt;"",MOD(L25+L26,360),"")</f>
         <v/>
       </c>
-      <c r="N25" s="28"/>
-      <c r="O25" s="12" t="str">
+      <c r="N25" s="150"/>
+      <c r="O25" s="196" t="str">
         <f>IF(ISNUMBER(I25),SQRT((H25^2) + (I25^2) - (2*H25*I25*COS(   ACOS(COS(RADIANS(J25-G25)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P25" s="12" t="str">
+      <c r="P25" s="196" t="str">
         <f>IF(ISNUMBER(O25),ROUND(N25/O25*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="15" t="str">
+      <c r="Q25" s="181"/>
+      <c r="R25" s="153" t="str">
         <f>IF(ISNUMBER(P25),P25*$R$10/60,"")</f>
         <v/>
       </c>
       <c r="S25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="T25" s="71"/>
-      <c r="U25" s="71"/>
+      <c r="T25" s="176"/>
+      <c r="U25" s="176"/>
       <c r="V25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="W25" s="71"/>
-      <c r="X25" s="154"/>
+      <c r="W25" s="176"/>
+      <c r="X25" s="177"/>
     </row>
     <row r="26" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="197"/>
-      <c r="B26" s="198"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="139"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="176"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="81"/>
-      <c r="J26" s="14" t="str">
+      <c r="D26" s="184"/>
+      <c r="E26" s="137"/>
+      <c r="F26" s="187"/>
+      <c r="G26" s="149"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="139"/>
+      <c r="J26" s="189" t="str">
         <f>IF(G25&lt;&gt;"",DEGREES(ASIN(H25/I25*SIN(RADIANS(G25-J25)))),"")</f>
         <v/>
       </c>
-      <c r="K26" s="29"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="143"/>
-      <c r="N26" s="14" t="str">
+      <c r="K26" s="151"/>
+      <c r="L26" s="153"/>
+      <c r="M26" s="193"/>
+      <c r="N26" s="189" t="str">
         <f>IF(ISNUMBER(N25),N24-N25,"")</f>
         <v/>
       </c>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="11" t="str">
+      <c r="O26" s="181"/>
+      <c r="P26" s="181"/>
+      <c r="Q26" s="181"/>
+      <c r="R26" s="197" t="str">
         <f>IF(AND(ISNUMBER(R24),ISNUMBER(R25)),R24-R25,"")</f>
         <v/>
       </c>
       <c r="S26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="T26" s="71"/>
-      <c r="U26" s="71"/>
+      <c r="T26" s="176"/>
+      <c r="U26" s="176"/>
       <c r="V26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="W26" s="71"/>
-      <c r="X26" s="154"/>
+      <c r="W26" s="176"/>
+      <c r="X26" s="177"/>
     </row>
     <row r="27" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="195"/>
-      <c r="B27" s="196"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="139" t="str">
+      <c r="A27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="184" t="str">
         <f>IF(J27&lt;&gt;"",MOD(J27+K28,360),"")</f>
         <v/>
       </c>
-      <c r="E27" s="140"/>
-      <c r="F27" s="201" t="str">
+      <c r="E27" s="137"/>
+      <c r="F27" s="186" t="str">
         <f t="shared" ref="F27" si="6">IF(ISNUMBER(E27),15-E27/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="12" t="str">
+      <c r="G27" s="150"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="139"/>
+      <c r="J27" s="150"/>
+      <c r="K27" s="196" t="str">
         <f>IF(J27&lt;&gt;"",IF(ISNUMBER(J28),MOD(J27+J28,360),J27),"")</f>
         <v/>
       </c>
-      <c r="L27" s="11" t="str">
+      <c r="L27" s="197" t="str">
         <f>IF(K27&lt;&gt;"",MOD(K27+K28,360),"")</f>
         <v/>
       </c>
-      <c r="M27" s="143" t="str">
+      <c r="M27" s="193" t="str">
         <f>IF(L27&lt;&gt;"",MOD(L27+L28,360),"")</f>
         <v/>
       </c>
-      <c r="N27" s="28"/>
-      <c r="O27" s="12" t="str">
+      <c r="N27" s="150"/>
+      <c r="O27" s="196" t="str">
         <f>IF(ISNUMBER(I27),SQRT((H27^2) + (I27^2) - (2*H27*I27*COS(   ACOS(COS(RADIANS(J27-G27)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P27" s="12" t="str">
+      <c r="P27" s="196" t="str">
         <f>IF(ISNUMBER(O27),ROUND(N27/O27*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="15" t="str">
+      <c r="Q27" s="181"/>
+      <c r="R27" s="153" t="str">
         <f>IF(ISNUMBER(P27),P27*$R$10/60,"")</f>
         <v/>
       </c>
       <c r="S27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="T27" s="71"/>
-      <c r="U27" s="71"/>
+      <c r="T27" s="176"/>
+      <c r="U27" s="176"/>
       <c r="V27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="W27" s="71"/>
-      <c r="X27" s="154"/>
+      <c r="W27" s="176"/>
+      <c r="X27" s="177"/>
     </row>
     <row r="28" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="197"/>
-      <c r="B28" s="198"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="139"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="176"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="81"/>
-      <c r="J28" s="14" t="str">
+      <c r="A28" s="45"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="187"/>
+      <c r="G28" s="149"/>
+      <c r="H28" s="138"/>
+      <c r="I28" s="139"/>
+      <c r="J28" s="189" t="str">
         <f>IF(G27&lt;&gt;"",DEGREES(ASIN(H27/I27*SIN(RADIANS(G27-J27)))),"")</f>
         <v/>
       </c>
-      <c r="K28" s="29"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="143"/>
-      <c r="N28" s="14" t="str">
+      <c r="K28" s="151"/>
+      <c r="L28" s="153"/>
+      <c r="M28" s="193"/>
+      <c r="N28" s="189" t="str">
         <f>IF(ISNUMBER(N27),N26-N27,"")</f>
         <v/>
       </c>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="11" t="str">
+      <c r="O28" s="181"/>
+      <c r="P28" s="181"/>
+      <c r="Q28" s="181"/>
+      <c r="R28" s="197" t="str">
         <f>IF(AND(ISNUMBER(R26),ISNUMBER(R27)),R26-R27,"")</f>
         <v/>
       </c>
       <c r="S28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="T28" s="71"/>
-      <c r="U28" s="71"/>
+      <c r="T28" s="176"/>
+      <c r="U28" s="176"/>
       <c r="V28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="W28" s="71"/>
-      <c r="X28" s="154"/>
+      <c r="W28" s="176"/>
+      <c r="X28" s="177"/>
     </row>
     <row r="29" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="195"/>
-      <c r="B29" s="196"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="139" t="str">
+      <c r="A29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="184" t="str">
         <f>IF(J29&lt;&gt;"",MOD(J29+K30,360),"")</f>
         <v/>
       </c>
-      <c r="E29" s="140"/>
-      <c r="F29" s="201" t="str">
+      <c r="E29" s="137"/>
+      <c r="F29" s="186" t="str">
         <f>IF(ISNUMBER(E29),15-E29/1000*2,"")</f>
         <v/>
       </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="12" t="str">
+      <c r="G29" s="150"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="196" t="str">
         <f>IF(J29&lt;&gt;"",IF(ISNUMBER(J30),MOD(J29+J30,360),J29),"")</f>
         <v/>
       </c>
-      <c r="L29" s="11" t="str">
+      <c r="L29" s="197" t="str">
         <f>IF(K29&lt;&gt;"",MOD(K29+K30,360),"")</f>
         <v/>
       </c>
-      <c r="M29" s="143" t="str">
+      <c r="M29" s="193" t="str">
         <f>IF(L29&lt;&gt;"",MOD(L29+L30,360),"")</f>
         <v/>
       </c>
-      <c r="N29" s="28"/>
-      <c r="O29" s="12" t="str">
+      <c r="N29" s="150"/>
+      <c r="O29" s="196" t="str">
         <f>IF(ISNUMBER(I29),SQRT((H29^2) + (I29^2) - (2*H29*I29*COS(   ACOS(COS(RADIANS(J29-G29)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P29" s="12" t="str">
+      <c r="P29" s="196" t="str">
         <f>IF(ISNUMBER(O29),ROUND(N29/O29*60,0),"")</f>
         <v/>
       </c>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="15" t="str">
+      <c r="Q29" s="181"/>
+      <c r="R29" s="153" t="str">
         <f>IF(ISNUMBER(P29),P29*$R$10/60,"")</f>
         <v/>
       </c>
       <c r="S29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="T29" s="71"/>
-      <c r="U29" s="71"/>
+      <c r="T29" s="176"/>
+      <c r="U29" s="176"/>
       <c r="V29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="W29" s="71"/>
-      <c r="X29" s="154"/>
+      <c r="W29" s="176"/>
+      <c r="X29" s="177"/>
     </row>
     <row r="30" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="197" t="s">
+      <c r="A30" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="198"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="139"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="176"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="80"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="14" t="str">
+      <c r="D30" s="184"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="187"/>
+      <c r="G30" s="149"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="139"/>
+      <c r="J30" s="189" t="str">
         <f>IF(G29&lt;&gt;"",DEGREES(ASIN(H29/I29*SIN(RADIANS(G29-J29)))),"")</f>
         <v/>
       </c>
-      <c r="K30" s="29"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="143"/>
-      <c r="N30" s="14" t="str">
+      <c r="K30" s="151"/>
+      <c r="L30" s="153"/>
+      <c r="M30" s="193"/>
+      <c r="N30" s="189" t="str">
         <f>IF(ISNUMBER(N29),N28-N29,"")</f>
         <v/>
       </c>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="11" t="str">
+      <c r="O30" s="181"/>
+      <c r="P30" s="181"/>
+      <c r="Q30" s="181"/>
+      <c r="R30" s="197" t="str">
         <f>IF(AND(ISNUMBER(R28),ISNUMBER(R29)),R28-R29,"")</f>
         <v/>
       </c>
       <c r="S30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="T30" s="71"/>
-      <c r="U30" s="71"/>
+      <c r="T30" s="176"/>
+      <c r="U30" s="176"/>
       <c r="V30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="W30" s="71"/>
-      <c r="X30" s="154"/>
+      <c r="W30" s="176"/>
+      <c r="X30" s="177"/>
     </row>
     <row r="31" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="195"/>
-      <c r="B31" s="196"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="139" t="str">
+      <c r="A31" s="43"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="184" t="str">
         <f>IF(J31&lt;&gt;"",MOD(J31+K32,360),"")</f>
         <v/>
       </c>
-      <c r="E31" s="140"/>
-      <c r="F31" s="176"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="81"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="12" t="str">
+      <c r="E31" s="137"/>
+      <c r="F31" s="187"/>
+      <c r="G31" s="150"/>
+      <c r="H31" s="151"/>
+      <c r="I31" s="139"/>
+      <c r="J31" s="150"/>
+      <c r="K31" s="196" t="str">
         <f>IF(J31&lt;&gt;"",IF(ISNUMBER(J32),MOD(J31+J32,360),J31),"")</f>
         <v/>
       </c>
-      <c r="L31" s="11" t="str">
+      <c r="L31" s="197" t="str">
         <f>IF(K31&lt;&gt;"",MOD(K31+K32,360),"")</f>
         <v/>
       </c>
-      <c r="M31" s="143" t="str">
+      <c r="M31" s="193" t="str">
         <f>IF(L31&lt;&gt;"",MOD(L31+L32,360),"")</f>
         <v/>
       </c>
-      <c r="N31" s="14" t="str">
+      <c r="N31" s="189" t="str">
         <f>IF(AND(ISNUMBER(O31),ISNUMBER(P31)),ROUND(P31*O31/60,0),"")</f>
         <v/>
       </c>
-      <c r="O31" s="12" t="str">
+      <c r="O31" s="196" t="str">
         <f>IF(ISNUMBER(I31),SQRT((H31^2) + (I31^2) - (2*H31*I31*COS(   ACOS(COS(RADIANS(J31-G31)))   ) ) ),"")</f>
         <v/>
       </c>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="15" t="str">
+      <c r="P31" s="151"/>
+      <c r="Q31" s="181"/>
+      <c r="R31" s="153" t="str">
         <f>IF(ISNUMBER(P31),P31*$R$10/60,"")</f>
         <v/>
       </c>
       <c r="S31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="T31" s="92"/>
-      <c r="U31" s="92"/>
+      <c r="T31" s="178"/>
+      <c r="U31" s="178"/>
       <c r="V31" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="W31" s="92"/>
-      <c r="X31" s="93"/>
+      <c r="W31" s="178"/>
+      <c r="X31" s="179"/>
     </row>
     <row r="32" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="197" t="s">
+      <c r="A32" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="198"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="166"/>
-      <c r="E32" s="167"/>
-      <c r="F32" s="177"/>
-      <c r="G32" s="202"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="14" t="str">
+      <c r="B32" s="46"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="185"/>
+      <c r="E32" s="142"/>
+      <c r="F32" s="188"/>
+      <c r="G32" s="152"/>
+      <c r="H32" s="143"/>
+      <c r="I32" s="144"/>
+      <c r="J32" s="189" t="str">
         <f>IF(G31&lt;&gt;"",DEGREES(ASIN(H31/I31*SIN(RADIANS(G31-J31)))),"")</f>
         <v/>
       </c>
-      <c r="K32" s="31"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="169"/>
-      <c r="N32" s="41" t="str">
+      <c r="K32" s="154"/>
+      <c r="L32" s="155"/>
+      <c r="M32" s="194"/>
+      <c r="N32" s="200" t="str">
         <f>IF(ISNUMBER(N31),N12-SUM(N13,N15,N17,N19,N21,N23,N25,N27,N29,N31),"")</f>
         <v/>
       </c>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="42" t="str">
+      <c r="O32" s="182"/>
+      <c r="P32" s="182"/>
+      <c r="Q32" s="182"/>
+      <c r="R32" s="199" t="str">
         <f>IF(AND(ISNUMBER(R30),ISNUMBER(R31)),R30-R31,"")</f>
         <v/>
       </c>
-      <c r="S32" s="157" t="s">
+      <c r="S32" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="T32" s="158"/>
-      <c r="U32" s="69"/>
-      <c r="V32" s="69"/>
-      <c r="W32" s="69" t="s">
+      <c r="T32" s="71"/>
+      <c r="U32" s="82"/>
+      <c r="V32" s="82"/>
+      <c r="W32" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="X32" s="70"/>
+      <c r="X32" s="119"/>
     </row>
     <row r="33" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="199"/>
-      <c r="B33" s="200"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="161" t="s">
+      <c r="A33" s="47"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="162"/>
-      <c r="F33" s="162"/>
-      <c r="G33" s="162"/>
-      <c r="H33" s="162"/>
-      <c r="I33" s="162"/>
-      <c r="J33" s="162"/>
-      <c r="K33" s="162"/>
-      <c r="L33" s="162"/>
-      <c r="M33" s="163"/>
-      <c r="N33" s="54">
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="27">
         <f>SUM(N13,N15,N17,N19,N21,N23,N25,N27,N29,N31)</f>
         <v>0</v>
       </c>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49">
+      <c r="O33" s="23"/>
+      <c r="P33" s="23">
         <f>SUM(P13,P15,P17,P19,P21,P23,P25,P27,P29,P31)</f>
         <v>0</v>
       </c>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="54">
+      <c r="Q33" s="23"/>
+      <c r="R33" s="27">
         <f>SUM(R13,R15,R17,R19,R21,R23,R25,R27,R29,R31)+$M$34</f>
         <v>0</v>
       </c>
-      <c r="S33" s="159" t="s">
+      <c r="S33" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="T33" s="160"/>
-      <c r="U33" s="156"/>
-      <c r="V33" s="156"/>
-      <c r="W33" s="156"/>
-      <c r="X33" s="165"/>
+      <c r="T33" s="73"/>
+      <c r="U33" s="67"/>
+      <c r="V33" s="67"/>
+      <c r="W33" s="67"/>
+      <c r="X33" s="81"/>
     </row>
     <row r="34" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="55"/>
-      <c r="C34" s="56" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="68"/>
-      <c r="E34" s="184" t="s">
+      <c r="D34" s="157"/>
+      <c r="E34" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="184"/>
-      <c r="G34" s="51"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="158"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="58" t="s">
+      <c r="I34" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="J34" s="57"/>
-      <c r="K34" s="192" t="s">
+      <c r="J34" s="159"/>
+      <c r="K34" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="L34" s="184"/>
-      <c r="M34" s="57"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="159"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="59" t="s">
+      <c r="P34" s="31" t="s">
         <v>62</v>
       </c>
       <c r="Q34" s="1"/>
-      <c r="R34" s="57"/>
+      <c r="R34" s="159"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-      <c r="U34" s="59" t="s">
+      <c r="U34" s="31" t="s">
         <v>63</v>
       </c>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="52"/>
+      <c r="X34" s="25"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="156" t="s">
         <v>75</v>
       </c>
       <c r="C35" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="183" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="9"/>
+      <c r="F35" s="183"/>
       <c r="G35" t="s">
         <v>81</v>
       </c>
-      <c r="L35" s="10" t="s">
+      <c r="L35" s="195" t="s">
         <v>79</v>
       </c>
       <c r="M35" t="s">
@@ -3760,65 +3760,102 @@
     </row>
   </sheetData>
   <mergeCells count="179">
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="M31:M32"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="W32:X32"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="S9:T10"/>
+    <mergeCell ref="U9:V10"/>
+    <mergeCell ref="W9:X10"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="S18:X18"/>
+    <mergeCell ref="S19:X19"/>
+    <mergeCell ref="S20:X20"/>
+    <mergeCell ref="W31:X31"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="O2:X8"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="H1:Q1"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="W29:X29"/>
+    <mergeCell ref="W30:X30"/>
+    <mergeCell ref="V22:X22"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U17:V17"/>
     <mergeCell ref="S32:T32"/>
     <mergeCell ref="S33:T33"/>
     <mergeCell ref="D33:M33"/>
@@ -3843,102 +3880,65 @@
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="W29:X29"/>
-    <mergeCell ref="W30:X30"/>
-    <mergeCell ref="V22:X22"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="H1:Q1"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="A9:B11"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="O2:X8"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="W32:X32"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="S9:T10"/>
-    <mergeCell ref="U9:V10"/>
-    <mergeCell ref="W9:X10"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="S18:X18"/>
-    <mergeCell ref="S19:X19"/>
-    <mergeCell ref="S20:X20"/>
-    <mergeCell ref="W31:X31"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G32:H32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="R1" r:id="rId1" xr:uid="{A3AF2B82-9261-4E31-AF70-31D3D7157CB2}"/>

</xml_diff>